<commit_message>
revisión sett recr dev con y sin flotas efecBo
</commit_message>
<xml_diff>
--- a/SETTING CASES.xlsx
+++ b/SETTING CASES.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>Stock-recluta</t>
   </si>
@@ -601,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,7 +621,7 @@
     <col min="3" max="3" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" style="2" customWidth="1"/>
     <col min="5" max="6" width="10.90625" style="2"/>
-    <col min="7" max="7" width="9.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.90625" style="2"/>
     <col min="12" max="16384" width="10.90625" style="2"/>
   </cols>
@@ -1270,6 +1270,12 @@
       <c r="D28" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
@@ -1285,7 +1291,15 @@
         <v>148.34299999999999</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2">
+        <v>156.92500000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
@@ -1301,7 +1315,15 @@
         <v>15.195399999999999</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="2">
+        <v>16.3627</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
@@ -1317,7 +1339,15 @@
         <v>122.295</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="2">
+        <v>130.047</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
@@ -1333,9 +1363,17 @@
         <v>0.95933599999999997</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="3">
+        <v>4</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.97024299999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>5</v>
       </c>
@@ -1349,9 +1387,17 @@
         <v>1.0004500000000001</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F33" s="3">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2.7384499999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>6</v>
       </c>
@@ -1365,9 +1411,17 @@
         <v>13.816000000000001</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="3">
+        <v>6</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="2">
+        <v>14.822900000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>7</v>
       </c>
@@ -1380,8 +1434,17 @@
       <c r="D35" s="17">
         <v>0.70157400000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F35" s="2">
+        <v>7</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.38007200000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>8</v>
       </c>
@@ -1395,9 +1458,17 @@
         <v>25</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.34071400000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -1410,8 +1481,17 @@
       <c r="D37" s="17">
         <v>0.27315800000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F37" s="2">
+        <v>9</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -1425,9 +1505,17 @@
         <v>37</v>
       </c>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F38" s="3">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -1441,9 +1529,17 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F39" s="3">
+        <v>11</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="2">
+        <v>2854.13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -1457,9 +1553,17 @@
         <v>685.697</v>
       </c>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F40" s="3">
+        <v>12</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.36743100000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>13</v>
       </c>
@@ -1473,9 +1577,17 @@
         <v>0.39672200000000002</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F41" s="3">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.46838800000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
revisando opciones de Forecast
</commit_message>
<xml_diff>
--- a/SETTING CASES.xlsx
+++ b/SETTING CASES.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SETTING" sheetId="9" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
   <si>
     <t>Stock-recluta</t>
   </si>
@@ -167,6 +168,12 @@
   </si>
   <si>
     <t>rev</t>
+  </si>
+  <si>
+    <t>Mod e y f</t>
+  </si>
+  <si>
+    <t>evaluan proyeccion con cambios en F.-</t>
   </si>
 </sst>
 </file>
@@ -601,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -611,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -1654,4 +1661,29 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>